<commit_message>
Added Image Printing For Excel Manager Prototype
</commit_message>
<xml_diff>
--- a/Project Files/Excel Manage Prototype/Text.xlsx
+++ b/Project Files/Excel Manage Prototype/Text.xlsx
@@ -90,6 +90,125 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="533400" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="533400" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="533400" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -415,5 +534,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Started Working On Exporting Sf2, MOre work on SF1
-Added field Birthplace Column on SF1... I forgot TEHEE :angel:
-Added getLetterValueAdvanced() Function for column addresses exceeding Z
</commit_message>
<xml_diff>
--- a/Project Files/Excel Manage Prototype/Text.xlsx
+++ b/Project Files/Excel Manage Prototype/Text.xlsx
@@ -508,7 +508,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A057ED4F-C60D-4A7F-A939-E81120426F1F}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:BA5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:E1"/>
@@ -528,7 +528,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="G5" t="s">
+      <c r="BA5" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>